<commit_message>
Rearranging files for final d-stats analysis
</commit_message>
<xml_diff>
--- a/OUT/PartitionedP_summaries.ANNOT_2022-11-16.xlsx
+++ b/OUT/PartitionedP_summaries.ANNOT_2022-11-16.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahipp\Documents\CODE\cerris-fdb\OUT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AAD1BB-1AAF-4ECE-9B18-F0DCE86C74DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F834CCED-C797-4CBC-B123-4F9872BBFF17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25455" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1579,7 +1579,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -2075,7 +2075,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2086,9 +2086,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2446,8 +2449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6291,32 +6294,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" s="3" t="s">
+    <row r="133" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="9" t="s">
         <v>507</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="C133" t="s">
-        <v>133</v>
-      </c>
-      <c r="D133" t="s">
+      <c r="C133" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D133" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E133">
+      <c r="E133" s="1">
         <v>400</v>
       </c>
-      <c r="F133" t="s">
+      <c r="F133" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="G133" t="s">
+      <c r="G133" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="H133" t="s">
+      <c r="H133" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="I133" s="7">
+      <c r="I133" s="6">
         <v>0.93</v>
       </c>
     </row>

</xml_diff>